<commit_message>
Object detection fully functional
</commit_message>
<xml_diff>
--- a/spreadsheets/OpenCV Calibration.xlsx
+++ b/spreadsheets/OpenCV Calibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajfar\Documents\Minibots\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B6A4E8-943B-4CE4-B560-ED16543D372A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF453E4-C7CD-48F1-8D45-72FA4124E4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EC02F603-D3F1-4AA6-8E07-64492A45B96D}"/>
   </bookViews>
@@ -995,7 +995,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>dist(cm) y=20</a:t>
+              <a:t>dist(cm) y=24</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5513,7 +5513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CF393F-B8E0-4547-9FE3-30BAAEA89E6A}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>

</xml_diff>